<commit_message>
QoL changes to .py and .ipynb
</commit_message>
<xml_diff>
--- a/app/data/241220_NfLPLADx_Plasma_demo/251006/241220_NfLPLADx_Plasma_demo.xlsx
+++ b/app/data/241220_NfLPLADx_Plasma_demo/251006/241220_NfLPLADx_Plasma_demo.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{E06BAA93-A5C0-8B44-A78C-82EB619886CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72BF2A92-912D-436B-92E1-F99D1E9369F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D99390B-9292-4C1E-BC74-DE0E0B893356}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D99390B-9292-4C1E-BC74-DE0E0B893356}"/>
   </bookViews>
   <sheets>
     <sheet name="e104" sheetId="1" r:id="rId1"/>
@@ -5779,8 +5779,8 @@
   </sheetPr>
   <dimension ref="A1:AR112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
QoL changes for imprecision calculation
</commit_message>
<xml_diff>
--- a/app/data/241220_NfLPLADx_Plasma_demo/251006/241220_NfLPLADx_Plasma_demo.xlsx
+++ b/app/data/241220_NfLPLADx_Plasma_demo/251006/241220_NfLPLADx_Plasma_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wehieduau-my.sharepoint.com/personal/smith_j_wehi_edu_au/Documents/Documents/Testing-Git/proxipal/app/data/241220_NfLPLADx_Plasma_demo/251006/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{E06BAA93-A5C0-8B44-A78C-82EB619886CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72BF2A92-912D-436B-92E1-F99D1E9369F1}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="13_ncr:1_{E06BAA93-A5C0-8B44-A78C-82EB619886CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A166AC5A-FFF9-4FB2-8B82-76060BD4B031}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D99390B-9292-4C1E-BC74-DE0E0B893356}"/>
   </bookViews>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="226">
   <si>
     <t>Experiment</t>
   </si>
@@ -5779,8 +5779,8 @@
   </sheetPr>
   <dimension ref="A1:AR112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6651,9 +6651,7 @@
       <c r="AH11" s="156" t="s">
         <v>197</v>
       </c>
-      <c r="AI11" s="141" t="s">
-        <v>219</v>
-      </c>
+      <c r="AI11" s="141"/>
       <c r="AK11" s="149" t="s">
         <v>212</v>
       </c>
@@ -13424,8 +13422,8 @@
       <c r="G77" s="25">
         <v>0.1</v>
       </c>
-      <c r="H77" s="50" t="str">
-        <v>unused</v>
+      <c r="H77" s="50">
+        <v>0</v>
       </c>
       <c r="I77" s="26"/>
       <c r="J77" s="27">

</xml_diff>